<commit_message>
made changes to format
</commit_message>
<xml_diff>
--- a/data/data_dictionary_current.xlsx
+++ b/data/data_dictionary_current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Maryland/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D373A40-32B1-F840-BC73-30CF832F5068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B1DD0C-AA2B-174D-A6F1-2174595B7B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="920" windowWidth="27840" windowHeight="17960" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="140" yWindow="760" windowWidth="27840" windowHeight="17240" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -143,9 +143,6 @@
     <t>Website</t>
   </si>
   <si>
-    <t>Sector</t>
-  </si>
-  <si>
     <t>label + percent</t>
   </si>
   <si>
@@ -1026,9 +1023,6 @@
     <t>Mission</t>
   </si>
   <si>
-    <t>Sector (Other)</t>
-  </si>
-  <si>
     <t>Organization Structure</t>
   </si>
   <si>
@@ -1405,6 +1399,12 @@
   </si>
   <si>
     <t>Professional Certification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sector </t>
+  </si>
+  <si>
+    <t>Organization Structure (Other)</t>
   </si>
 </sst>
 </file>
@@ -2317,305 +2317,305 @@
         <v>1</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="71" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="G2" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>58</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="E8" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="E14" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="D15" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="E16" s="11" t="s">
         <v>84</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="D17" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="E18" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2637,8 +2637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09851FDF-4334-4E44-81EF-4155DEF57BA3}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3293,7 +3293,7 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -3325,7 +3325,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
@@ -3389,7 +3389,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -3421,10 +3421,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D7" s="2">
         <v>8</v>
@@ -3453,10 +3453,10 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" s="2">
         <v>9</v>
@@ -3485,10 +3485,10 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D9" s="2">
         <v>10</v>
@@ -3517,10 +3517,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D10" s="2">
         <v>11</v>
@@ -3549,10 +3549,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D11" s="2">
         <v>12</v>
@@ -3581,10 +3581,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D12" s="2">
         <v>3</v>
@@ -3613,7 +3613,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>19</v>
@@ -3645,10 +3645,10 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D14" s="2">
         <v>14</v>
@@ -3677,10 +3677,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D15" s="2">
         <v>15</v>
@@ -3709,10 +3709,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D16" s="2">
         <v>16</v>
@@ -3741,10 +3741,10 @@
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D17" s="2">
         <v>2</v>
@@ -3773,10 +3773,10 @@
         <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>306</v>
       </c>
       <c r="D18" s="2">
         <v>17</v>
@@ -3794,7 +3794,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J18" s="2">
         <v>0</v>
@@ -3808,10 +3808,10 @@
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>307</v>
+        <v>433</v>
       </c>
       <c r="D19" s="2">
         <v>18</v>
@@ -3841,10 +3841,10 @@
         <v>11</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>308</v>
+        <v>432</v>
       </c>
       <c r="D20" s="2">
         <v>19</v>
@@ -3874,10 +3874,10 @@
         <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D21" s="2">
         <v>20</v>
@@ -3889,7 +3889,7 @@
         <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H21" s="2">
         <v>0</v>
@@ -3907,10 +3907,10 @@
         <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="2">
         <v>21</v>
@@ -3928,7 +3928,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J22" s="2">
         <v>0</v>
@@ -3942,10 +3942,10 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="2">
         <v>22</v>
@@ -3974,10 +3974,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D24" s="2">
         <v>23</v>
@@ -4006,10 +4006,10 @@
         <v>11</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D25" s="2">
         <v>24</v>
@@ -4038,10 +4038,10 @@
         <v>11</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D26" s="2">
         <v>25</v>
@@ -4070,10 +4070,10 @@
         <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D27" s="2">
         <v>26</v>
@@ -4102,10 +4102,10 @@
         <v>11</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D28" s="2">
         <v>27</v>
@@ -4134,10 +4134,10 @@
         <v>11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D29" s="2">
         <v>28</v>
@@ -4166,10 +4166,10 @@
         <v>11</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D30" s="2">
         <v>29</v>
@@ -4198,10 +4198,10 @@
         <v>11</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D31" s="2">
         <v>30</v>
@@ -4230,10 +4230,10 @@
         <v>11</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D32" s="2">
         <v>31</v>
@@ -4262,10 +4262,10 @@
         <v>11</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D33" s="2">
         <v>32</v>
@@ -4294,10 +4294,10 @@
         <v>11</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D34" s="2">
         <v>33</v>
@@ -4326,10 +4326,10 @@
         <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D35" s="2">
         <v>34</v>
@@ -4358,10 +4358,10 @@
         <v>11</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D36" s="2">
         <v>35</v>
@@ -4390,10 +4390,10 @@
         <v>11</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D37" s="2">
         <v>36</v>
@@ -4422,10 +4422,10 @@
         <v>11</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D38" s="2">
         <v>37</v>
@@ -4454,10 +4454,10 @@
         <v>11</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D39" s="2">
         <v>38</v>
@@ -4486,10 +4486,10 @@
         <v>11</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D40" s="2">
         <v>39</v>
@@ -4518,10 +4518,10 @@
         <v>11</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D41" s="2">
         <v>40</v>
@@ -4550,10 +4550,10 @@
         <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D42" s="2">
         <v>41</v>
@@ -4582,10 +4582,10 @@
         <v>11</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D43" s="2">
         <v>42</v>
@@ -4614,10 +4614,10 @@
         <v>11</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D44" s="2">
         <v>43</v>
@@ -4646,10 +4646,10 @@
         <v>11</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D45" s="2">
         <v>44</v>
@@ -4678,10 +4678,10 @@
         <v>11</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D46" s="2">
         <v>45</v>
@@ -4710,10 +4710,10 @@
         <v>11</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D47" s="2">
         <v>46</v>
@@ -4742,10 +4742,10 @@
         <v>11</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D48" s="2">
         <v>47</v>
@@ -4774,10 +4774,10 @@
         <v>11</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D49" s="2">
         <v>48</v>
@@ -4806,10 +4806,10 @@
         <v>11</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D50" s="2">
         <v>49</v>
@@ -4838,10 +4838,10 @@
         <v>11</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D51" s="2">
         <v>50</v>
@@ -4870,10 +4870,10 @@
         <v>11</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D52" s="2">
         <v>51</v>
@@ -4902,10 +4902,10 @@
         <v>11</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D53" s="2">
         <v>52</v>
@@ -4934,10 +4934,10 @@
         <v>11</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D54" s="2">
         <v>53</v>
@@ -4966,10 +4966,10 @@
         <v>11</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D55" s="2">
         <v>54</v>
@@ -4998,10 +4998,10 @@
         <v>11</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D56" s="2">
         <v>55</v>
@@ -5030,10 +5030,10 @@
         <v>11</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D57" s="2">
         <v>56</v>
@@ -5062,10 +5062,10 @@
         <v>11</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D58" s="2">
         <v>57</v>
@@ -5094,10 +5094,10 @@
         <v>11</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D59" s="2">
         <v>58</v>
@@ -5126,10 +5126,10 @@
         <v>11</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D60" s="2">
         <v>59</v>
@@ -5158,10 +5158,10 @@
         <v>11</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D61" s="2">
         <v>60</v>
@@ -5190,10 +5190,10 @@
         <v>11</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D62" s="2">
         <v>61</v>
@@ -5222,10 +5222,10 @@
         <v>11</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D63" s="2">
         <v>62</v>
@@ -5254,10 +5254,10 @@
         <v>11</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D64" s="2">
         <v>63</v>
@@ -5286,10 +5286,10 @@
         <v>11</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D65" s="2">
         <v>64</v>
@@ -5318,10 +5318,10 @@
         <v>11</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D66" s="2">
         <v>65</v>
@@ -5350,10 +5350,10 @@
         <v>11</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D67" s="2">
         <v>66</v>
@@ -5382,10 +5382,10 @@
         <v>11</v>
       </c>
       <c r="B68" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D68" s="2">
         <v>67</v>
@@ -5414,10 +5414,10 @@
         <v>11</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D69" s="2">
         <v>68</v>
@@ -5446,10 +5446,10 @@
         <v>11</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D70" s="2">
         <v>69</v>
@@ -5475,13 +5475,13 @@
     </row>
     <row r="71" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="C71" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="D71" s="2">
         <v>1</v>
@@ -5507,16 +5507,16 @@
     </row>
     <row r="72" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D72" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>14</v>
@@ -5539,16 +5539,16 @@
     </row>
     <row r="73" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D73" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>13</v>
@@ -5571,16 +5571,16 @@
     </row>
     <row r="74" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D74" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>13</v>
@@ -5603,16 +5603,16 @@
     </row>
     <row r="75" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D75" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>13</v>
@@ -5635,7 +5635,7 @@
     </row>
     <row r="76" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>12</v>
@@ -5644,7 +5644,7 @@
         <v>12</v>
       </c>
       <c r="D76" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>13</v>
@@ -5667,13 +5667,13 @@
     </row>
     <row r="77" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D77" s="2">
         <v>7</v>
@@ -5699,13 +5699,13 @@
     </row>
     <row r="78" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D78" s="4">
         <v>8</v>
@@ -5731,13 +5731,13 @@
     </row>
     <row r="79" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D79" s="2">
         <v>9</v>
@@ -5763,13 +5763,13 @@
     </row>
     <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D80" s="4">
         <v>10</v>
@@ -5795,13 +5795,13 @@
     </row>
     <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D81" s="2">
         <v>11</v>
@@ -5827,13 +5827,13 @@
     </row>
     <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D82" s="4">
         <v>12</v>
@@ -5859,13 +5859,13 @@
     </row>
     <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D83" s="2">
         <v>13</v>
@@ -5891,13 +5891,13 @@
     </row>
     <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D84" s="4">
         <v>14</v>
@@ -5923,13 +5923,13 @@
     </row>
     <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D85" s="2">
         <v>15</v>
@@ -5955,13 +5955,13 @@
     </row>
     <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="D86" s="4">
         <v>16</v>
@@ -5987,13 +5987,13 @@
     </row>
     <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D87" s="2">
         <v>17</v>
@@ -6019,13 +6019,13 @@
     </row>
     <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D88" s="4">
         <v>18</v>
@@ -6051,13 +6051,13 @@
     </row>
     <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D89" s="2">
         <v>19</v>
@@ -6083,13 +6083,13 @@
     </row>
     <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D90" s="4">
         <v>20</v>
@@ -6115,13 +6115,13 @@
     </row>
     <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D91" s="2">
         <v>21</v>
@@ -6147,13 +6147,13 @@
     </row>
     <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D92" s="4">
         <v>22</v>
@@ -6179,13 +6179,13 @@
     </row>
     <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D93" s="2">
         <v>23</v>
@@ -6211,13 +6211,13 @@
     </row>
     <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D94" s="4">
         <v>24</v>
@@ -6243,13 +6243,13 @@
     </row>
     <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D95" s="2">
         <v>25</v>
@@ -6275,13 +6275,13 @@
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D96" s="4">
         <v>26</v>
@@ -6307,13 +6307,13 @@
     </row>
     <row r="97" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D97" s="2">
         <v>27</v>
@@ -6339,13 +6339,13 @@
     </row>
     <row r="98" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D98" s="4">
         <v>28</v>
@@ -6371,13 +6371,13 @@
     </row>
     <row r="99" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D99" s="2">
         <v>29</v>
@@ -6403,13 +6403,13 @@
     </row>
     <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D100" s="4">
         <v>30</v>
@@ -6435,13 +6435,13 @@
     </row>
     <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D101" s="2">
         <v>31</v>
@@ -6467,13 +6467,13 @@
     </row>
     <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D102" s="4">
         <v>32</v>
@@ -6499,13 +6499,13 @@
     </row>
     <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D103" s="2">
         <v>33</v>
@@ -6531,13 +6531,13 @@
     </row>
     <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D104" s="4">
         <v>34</v>
@@ -6563,13 +6563,13 @@
     </row>
     <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D105" s="2">
         <v>35</v>
@@ -6595,13 +6595,13 @@
     </row>
     <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D106" s="4">
         <v>36</v>
@@ -6627,13 +6627,13 @@
     </row>
     <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D107" s="2">
         <v>37</v>
@@ -6659,13 +6659,13 @@
     </row>
     <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D108" s="4">
         <v>38</v>
@@ -6691,13 +6691,13 @@
     </row>
     <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D109" s="2">
         <v>39</v>
@@ -6723,13 +6723,13 @@
     </row>
     <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D110" s="4">
         <v>40</v>
@@ -6755,13 +6755,13 @@
     </row>
     <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D111" s="2">
         <v>41</v>
@@ -6787,13 +6787,13 @@
     </row>
     <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D112" s="4">
         <v>42</v>
@@ -6819,13 +6819,13 @@
     </row>
     <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D113" s="2">
         <v>43</v>
@@ -6851,13 +6851,13 @@
     </row>
     <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D114" s="4">
         <v>44</v>
@@ -6883,13 +6883,13 @@
     </row>
     <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D115" s="2">
         <v>45</v>
@@ -6915,13 +6915,13 @@
     </row>
     <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D116" s="4">
         <v>46</v>
@@ -6947,13 +6947,13 @@
     </row>
     <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B117" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D117" s="2">
         <v>47</v>
@@ -7003,7 +7003,7 @@
   <dimension ref="A1:N119"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7594,13 +7594,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -7608,13 +7608,13 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -7631,13 +7631,13 @@
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -7648,13 +7648,13 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="2">
         <v>3</v>
@@ -7665,13 +7665,13 @@
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="2">
         <v>4</v>
@@ -7682,13 +7682,13 @@
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E6" s="2">
         <v>5</v>
@@ -7699,13 +7699,13 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="2">
         <v>6</v>
@@ -7716,13 +7716,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E8" s="2">
         <v>7</v>
@@ -7733,13 +7733,13 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
@@ -7750,13 +7750,13 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E10" s="2">
         <v>9</v>
@@ -7767,13 +7767,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E11" s="2">
         <v>10</v>
@@ -7784,13 +7784,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12" s="2">
         <v>11</v>
@@ -7801,13 +7801,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" s="2">
         <v>12</v>
@@ -7818,13 +7818,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E14" s="2">
         <v>1</v>
@@ -7835,13 +7835,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E15" s="2">
         <v>2</v>
@@ -7852,13 +7852,13 @@
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E16" s="2">
         <v>3</v>
@@ -7869,13 +7869,13 @@
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C17" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="E17" s="2">
         <v>4</v>
@@ -7886,13 +7886,13 @@
         <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C18" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="E18" s="2">
         <v>5</v>
@@ -7903,13 +7903,13 @@
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" s="2">
         <v>6</v>
@@ -7920,13 +7920,13 @@
         <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="E20" s="2">
         <v>1</v>
@@ -7937,13 +7937,13 @@
         <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="E21" s="2">
         <v>2</v>
@@ -7954,13 +7954,13 @@
         <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C22" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="E22" s="2">
         <v>3</v>
@@ -7971,13 +7971,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="E23" s="2">
         <v>4</v>
@@ -7988,13 +7988,13 @@
         <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E24" s="2">
         <v>5</v>
@@ -8005,13 +8005,13 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="2">
         <v>1</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
@@ -8022,13 +8022,13 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="2">
         <v>2</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E26" s="2">
         <v>2</v>
@@ -8039,13 +8039,13 @@
         <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" s="2">
         <v>3</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E27" s="2">
         <v>3</v>
@@ -8056,13 +8056,13 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" s="2">
         <v>4</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E28" s="2">
         <v>4</v>
@@ -8073,13 +8073,13 @@
         <v>11</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" s="2">
         <v>5</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E29" s="2">
         <v>5</v>
@@ -8090,13 +8090,13 @@
         <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="2">
         <v>6</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E30" s="2">
         <v>6</v>
@@ -8107,13 +8107,13 @@
         <v>11</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="2">
         <v>7</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E31" s="2">
         <v>7</v>
@@ -8124,13 +8124,13 @@
         <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="2">
         <v>8</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E32" s="2">
         <v>8</v>
@@ -8141,13 +8141,13 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2">
         <v>9</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E33" s="2">
         <v>9</v>
@@ -8158,13 +8158,13 @@
         <v>11</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E34" s="2">
         <v>10</v>
@@ -8175,13 +8175,13 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E35" s="2">
         <v>1</v>
@@ -8192,13 +8192,13 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E36" s="2">
         <v>2</v>
@@ -8209,13 +8209,13 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E37" s="2">
         <v>3</v>
@@ -8226,13 +8226,13 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E38" s="2">
         <v>4</v>
@@ -8243,13 +8243,13 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E39" s="2">
         <v>5</v>
@@ -8260,13 +8260,13 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E40" s="2">
         <v>6</v>
@@ -8277,13 +8277,13 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E41" s="2">
         <v>7</v>
@@ -8294,13 +8294,13 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E42" s="2">
         <v>8</v>
@@ -8311,13 +8311,13 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E43" s="2">
         <v>9</v>
@@ -8328,13 +8328,13 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E44" s="2">
         <v>10</v>
@@ -8345,13 +8345,13 @@
         <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E45" s="2">
         <v>11</v>
@@ -8362,13 +8362,13 @@
         <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E46" s="2">
         <v>12</v>
@@ -8379,13 +8379,13 @@
         <v>11</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E47" s="2">
         <v>1</v>
@@ -8396,13 +8396,13 @@
         <v>11</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
@@ -8413,13 +8413,13 @@
         <v>11</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E49" s="2">
         <v>3</v>
@@ -8430,13 +8430,13 @@
         <v>11</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E50" s="2">
         <v>4</v>
@@ -8447,13 +8447,13 @@
         <v>11</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E51" s="2">
         <v>5</v>
@@ -8464,13 +8464,13 @@
         <v>11</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E52" s="2">
         <v>6</v>
@@ -8481,13 +8481,13 @@
         <v>11</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E53" s="2">
         <v>7</v>
@@ -8498,13 +8498,13 @@
         <v>11</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E54" s="2">
         <v>8</v>
@@ -8515,13 +8515,13 @@
         <v>11</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E55" s="2">
         <v>9</v>
@@ -8532,13 +8532,13 @@
         <v>11</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="E56" s="2">
         <v>10</v>
@@ -8549,13 +8549,13 @@
         <v>11</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="E57" s="2">
         <v>11</v>
@@ -8563,10 +8563,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>13</v>
@@ -8580,10 +8580,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>14</v>
@@ -8597,16 +8597,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E60" s="2">
         <v>1</v>
@@ -8614,16 +8614,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E61" s="2">
         <v>2</v>
@@ -8631,16 +8631,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E62" s="2">
         <v>3</v>
@@ -8648,16 +8648,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E63" s="2">
         <v>4</v>
@@ -8665,16 +8665,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E64" s="2">
         <v>5</v>
@@ -8682,16 +8682,16 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E65" s="2">
         <v>1</v>
@@ -8701,16 +8701,16 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E66" s="2">
         <v>2</v>
@@ -8720,16 +8720,16 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E67" s="2">
         <v>3</v>
@@ -8737,16 +8737,16 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E68" s="2">
         <v>4</v>
@@ -8754,16 +8754,16 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E69" s="2">
         <v>5</v>
@@ -8771,16 +8771,16 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E70" s="2">
         <v>6</v>
@@ -8788,16 +8788,16 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E71" s="2">
         <v>7</v>
@@ -8805,16 +8805,16 @@
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E72" s="2">
         <v>8</v>
@@ -8822,16 +8822,16 @@
     </row>
     <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E73" s="2">
         <v>9</v>
@@ -8848,16 +8848,16 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E74" s="2">
         <v>10</v>
@@ -8865,16 +8865,16 @@
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E75" s="2">
         <v>11</v>
@@ -8882,16 +8882,16 @@
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E76" s="2">
         <v>12</v>
@@ -8899,16 +8899,16 @@
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E77" s="2">
         <v>13</v>
@@ -8916,16 +8916,16 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E78" s="2">
         <v>14</v>
@@ -8933,16 +8933,16 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E79" s="2">
         <v>1</v>
@@ -8950,16 +8950,16 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E80" s="2">
         <v>2</v>
@@ -8967,16 +8967,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C81" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D81" s="17" t="s">
         <v>151</v>
-      </c>
-      <c r="D81" s="17" t="s">
-        <v>152</v>
       </c>
       <c r="E81" s="2">
         <v>3</v>
@@ -8984,16 +8984,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C82" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D82" s="17" t="s">
         <v>153</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>154</v>
       </c>
       <c r="E82" s="2">
         <v>4</v>
@@ -9001,16 +9001,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C83" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D83" s="17" t="s">
         <v>155</v>
-      </c>
-      <c r="D83" s="17" t="s">
-        <v>156</v>
       </c>
       <c r="E83" s="2">
         <v>5</v>
@@ -9018,16 +9018,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C84" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D84" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="E84" s="2">
         <v>6</v>
@@ -9035,16 +9035,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C85" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D85" s="17" t="s">
         <v>159</v>
-      </c>
-      <c r="D85" s="17" t="s">
-        <v>160</v>
       </c>
       <c r="E85" s="2">
         <v>7</v>
@@ -9052,16 +9052,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C86" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D86" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="D86" s="17" t="s">
-        <v>162</v>
       </c>
       <c r="E86" s="2">
         <v>8</v>
@@ -9069,16 +9069,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C87" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D87" s="17" t="s">
         <v>163</v>
-      </c>
-      <c r="D87" s="17" t="s">
-        <v>164</v>
       </c>
       <c r="E87" s="2">
         <v>9</v>
@@ -9086,16 +9086,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C88" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D88" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="D88" s="17" t="s">
-        <v>166</v>
       </c>
       <c r="E88" s="2">
         <v>10</v>
@@ -9103,16 +9103,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C89" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D89" s="17" t="s">
         <v>167</v>
-      </c>
-      <c r="D89" s="17" t="s">
-        <v>168</v>
       </c>
       <c r="E89" s="2">
         <v>11</v>
@@ -9120,16 +9120,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C90" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D90" s="17" t="s">
         <v>169</v>
-      </c>
-      <c r="D90" s="17" t="s">
-        <v>170</v>
       </c>
       <c r="E90" s="2">
         <v>12</v>
@@ -9137,16 +9137,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C91" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D91" s="17" t="s">
         <v>171</v>
-      </c>
-      <c r="D91" s="17" t="s">
-        <v>172</v>
       </c>
       <c r="E91" s="2">
         <v>13</v>
@@ -9154,16 +9154,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C92" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D92" s="17" t="s">
         <v>173</v>
-      </c>
-      <c r="D92" s="17" t="s">
-        <v>174</v>
       </c>
       <c r="E92" s="2">
         <v>14</v>
@@ -9171,16 +9171,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E93" s="2">
         <v>15</v>
@@ -9188,16 +9188,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E94" s="2">
         <v>16</v>
@@ -9205,16 +9205,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E95" s="2">
         <v>17</v>
@@ -9222,16 +9222,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C96" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D96" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>179</v>
       </c>
       <c r="E96" s="2">
         <v>18</v>
@@ -9239,16 +9239,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C97" t="s">
+        <v>179</v>
+      </c>
+      <c r="D97" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="E97" s="2">
         <v>1</v>
@@ -9256,16 +9256,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E98" s="2">
         <v>2</v>
@@ -9273,16 +9273,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E99" s="2">
         <v>3</v>
@@ -9290,16 +9290,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E100" s="2">
         <v>1</v>
@@ -9307,16 +9307,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E101" s="2">
         <v>2</v>
@@ -9324,16 +9324,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E102" s="2">
         <v>3</v>
@@ -9341,16 +9341,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E103" s="2">
         <v>4</v>
@@ -9358,16 +9358,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E104" s="2">
         <v>5</v>
@@ -9375,16 +9375,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E105" s="2">
         <v>6</v>
@@ -9392,16 +9392,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="E106" s="2">
         <v>1</v>
@@ -9409,16 +9409,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="E107" s="2">
         <v>2</v>
@@ -9426,16 +9426,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="E108" s="2">
         <v>3</v>
@@ -9443,16 +9443,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="E109" s="2">
         <v>4</v>
@@ -9460,16 +9460,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="E110" s="2">
         <v>5</v>
@@ -9477,16 +9477,16 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E111" s="2">
         <v>6</v>
@@ -9494,16 +9494,16 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="E112" s="2">
         <v>7</v>
@@ -9511,16 +9511,16 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E113" s="2">
         <v>8</v>
@@ -9528,16 +9528,16 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D114" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E114" s="2">
         <v>9</v>
@@ -9545,16 +9545,16 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E115" s="2">
         <v>10</v>
@@ -9562,16 +9562,16 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E116" s="2">
         <v>11</v>
@@ -9579,16 +9579,16 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E117" s="2">
         <v>12</v>
@@ -9596,16 +9596,16 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E118" s="2">
         <v>13</v>
@@ -9613,16 +9613,16 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E119" s="2">
         <v>14</v>

</xml_diff>

<commit_message>
added a new filter
</commit_message>
<xml_diff>
--- a/data/data_dictionary_current.xlsx
+++ b/data/data_dictionary_current.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gpain/Documents/Work_Dashboards/Maryland/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B1DD0C-AA2B-174D-A6F1-2174595B7B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDE3EEC-BFDA-944F-8F0F-F3CD51B1D081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="760" windowWidth="27840" windowHeight="17240" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
+    <workbookView xWindow="15180" yWindow="920" windowWidth="14900" windowHeight="16920" activeTab="1" xr2:uid="{949A1E6F-A50E-0D47-B806-7BF7EBA35A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="2" r:id="rId1"/>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="443">
   <si>
     <t>table_name</t>
   </si>
@@ -1405,6 +1405,33 @@
   </si>
   <si>
     <t>Organization Structure (Other)</t>
+  </si>
+  <si>
+    <t>Independently-operating organization</t>
+  </si>
+  <si>
+    <t>Department within large institution (city | university | etc.)</t>
+  </si>
+  <si>
+    <t>Chapter/regional office operating under a parent entity</t>
+  </si>
+  <si>
+    <t>Parent entity/headquarters</t>
+  </si>
+  <si>
+    <t>org-structure-other</t>
+  </si>
+  <si>
+    <t>Independently Operated Org.</t>
+  </si>
+  <si>
+    <t>Large Institution</t>
+  </si>
+  <si>
+    <t>Parent Entity</t>
+  </si>
+  <si>
+    <t>Chapter/Regional Office</t>
   </si>
 </sst>
 </file>
@@ -2637,8 +2664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09851FDF-4334-4E44-81EF-4155DEF57BA3}">
   <dimension ref="A1:K122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3856,17 +3883,19 @@
         <v>13</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="2">
-        <v>0</v>
-      </c>
-      <c r="I20" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="J20" s="2">
         <v>0</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -7000,10 +7029,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D1373AD-CAFE-FC46-B12F-4E16ECB9F9F7}">
-  <dimension ref="A1:N119"/>
+  <dimension ref="A1:N124"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A34" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8563,16 +8592,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>38</v>
+        <v>210</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>13</v>
+        <v>434</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>13</v>
+        <v>439</v>
       </c>
       <c r="E58" s="2">
         <v>1</v>
@@ -8580,16 +8609,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>38</v>
+        <v>210</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>14</v>
+        <v>435</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>14</v>
+        <v>440</v>
       </c>
       <c r="E59" s="2">
         <v>2</v>
@@ -8597,53 +8626,53 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>271</v>
+        <v>210</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>131</v>
+        <v>436</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>131</v>
+        <v>442</v>
       </c>
       <c r="E60" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>271</v>
+        <v>210</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>132</v>
+        <v>437</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>132</v>
+        <v>441</v>
       </c>
       <c r="E61" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>271</v>
+        <v>210</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>133</v>
+        <v>438</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="E62" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -8651,16 +8680,16 @@
         <v>29</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>271</v>
+        <v>38</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>134</v>
+        <v>13</v>
       </c>
       <c r="E63" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
@@ -8668,68 +8697,64 @@
         <v>29</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>271</v>
+        <v>38</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
       <c r="E64" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="14" t="s">
-        <v>263</v>
+      <c r="B65" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E65" s="2">
         <v>1</v>
       </c>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B66" s="14" t="s">
-        <v>263</v>
+      <c r="B66" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E66" s="2">
         <v>2</v>
       </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B67" s="14" t="s">
-        <v>263</v>
+      <c r="B67" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E67" s="2">
         <v>3</v>
@@ -8739,14 +8764,14 @@
       <c r="A68" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="14" t="s">
-        <v>263</v>
+      <c r="B68" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="E68" s="2">
         <v>4</v>
@@ -8756,14 +8781,14 @@
       <c r="A69" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B69" s="14" t="s">
-        <v>263</v>
+      <c r="B69" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E69" s="2">
         <v>5</v>
@@ -8777,14 +8802,16 @@
         <v>263</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E70" s="2">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
@@ -8794,14 +8821,16 @@
         <v>263</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E71" s="2">
-        <v>7</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
@@ -8811,16 +8840,16 @@
         <v>263</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E72" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>29</v>
       </c>
@@ -8828,23 +8857,14 @@
         <v>263</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="E73" s="2">
-        <v>9</v>
-      </c>
-      <c r="F73" s="16"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-      <c r="K73" s="2"/>
-      <c r="L73" s="2"/>
-      <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
@@ -8854,13 +8874,13 @@
         <v>263</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E74" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -8871,13 +8891,13 @@
         <v>263</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E75" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -8888,13 +8908,13 @@
         <v>263</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E76" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -8905,16 +8925,16 @@
         <v>263</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E77" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>29</v>
       </c>
@@ -8922,30 +8942,39 @@
         <v>263</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="E78" s="2">
-        <v>14</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F78" s="16"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E79" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -8953,16 +8982,16 @@
         <v>29</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>149</v>
+        <v>263</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="E80" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
@@ -8970,16 +8999,16 @@
         <v>29</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D81" s="17" t="s">
-        <v>151</v>
+        <v>263</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="E81" s="2">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
@@ -8987,16 +9016,16 @@
         <v>29</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>153</v>
+        <v>263</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="E82" s="2">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
@@ -9004,16 +9033,16 @@
         <v>29</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="D83" s="17" t="s">
-        <v>155</v>
+        <v>263</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="E83" s="2">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
@@ -9023,14 +9052,14 @@
       <c r="B84" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C84" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>157</v>
+      <c r="C84" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="E84" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -9041,13 +9070,13 @@
         <v>269</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E85" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
@@ -9058,13 +9087,13 @@
         <v>269</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E86" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
@@ -9075,13 +9104,13 @@
         <v>269</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="E87" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
@@ -9092,13 +9121,13 @@
         <v>269</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="E88" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -9109,13 +9138,13 @@
         <v>269</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="E89" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
@@ -9126,13 +9155,13 @@
         <v>269</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D90" s="17" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E90" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
@@ -9143,13 +9172,13 @@
         <v>269</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D91" s="17" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="E91" s="2">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -9160,13 +9189,13 @@
         <v>269</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="E92" s="2">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
@@ -9176,14 +9205,14 @@
       <c r="B93" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C93" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>174</v>
+      <c r="C93" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D93" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="E93" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
@@ -9193,14 +9222,14 @@
       <c r="B94" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>175</v>
+      <c r="C94" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D94" s="17" t="s">
+        <v>167</v>
       </c>
       <c r="E94" s="2">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
@@ -9210,14 +9239,14 @@
       <c r="B95" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>176</v>
+      <c r="C95" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D95" s="17" t="s">
+        <v>169</v>
       </c>
       <c r="E95" s="2">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
@@ -9227,14 +9256,14 @@
       <c r="B96" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>178</v>
+      <c r="C96" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D96" s="17" t="s">
+        <v>171</v>
       </c>
       <c r="E96" s="2">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
@@ -9242,16 +9271,16 @@
         <v>29</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="C97" t="s">
-        <v>179</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>180</v>
+        <v>269</v>
+      </c>
+      <c r="C97" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="D97" s="17" t="s">
+        <v>173</v>
       </c>
       <c r="E97" s="2">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
@@ -9259,16 +9288,16 @@
         <v>29</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E98" s="2">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
@@ -9276,16 +9305,16 @@
         <v>29</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E99" s="2">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
@@ -9293,16 +9322,16 @@
         <v>29</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E100" s="2">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
@@ -9310,16 +9339,16 @@
         <v>29</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E101" s="2">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
@@ -9327,16 +9356,16 @@
         <v>29</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>185</v>
+        <v>278</v>
+      </c>
+      <c r="C102" t="s">
+        <v>179</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E102" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
@@ -9344,16 +9373,16 @@
         <v>29</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E103" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
@@ -9361,16 +9390,16 @@
         <v>29</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E104" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
@@ -9381,13 +9410,13 @@
         <v>279</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
       <c r="E105" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
@@ -9395,16 +9424,16 @@
         <v>29</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>409</v>
+        <v>184</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>410</v>
+        <v>184</v>
       </c>
       <c r="E106" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
@@ -9412,16 +9441,16 @@
         <v>29</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>411</v>
+        <v>185</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>412</v>
+        <v>185</v>
       </c>
       <c r="E107" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
@@ -9429,16 +9458,16 @@
         <v>29</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>413</v>
+        <v>186</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>414</v>
+        <v>186</v>
       </c>
       <c r="E108" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
@@ -9446,16 +9475,16 @@
         <v>29</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>415</v>
+        <v>187</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>416</v>
+        <v>187</v>
       </c>
       <c r="E109" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -9463,16 +9492,16 @@
         <v>29</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>259</v>
+        <v>279</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>417</v>
+        <v>103</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>418</v>
+        <v>103</v>
       </c>
       <c r="E110" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
@@ -9483,13 +9512,13 @@
         <v>259</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="E111" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
@@ -9500,13 +9529,13 @@
         <v>259</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="E112" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
@@ -9517,13 +9546,13 @@
         <v>259</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="E113" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
@@ -9534,13 +9563,13 @@
         <v>259</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="D114" t="s">
-        <v>425</v>
+        <v>415</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>416</v>
       </c>
       <c r="E114" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
@@ -9551,13 +9580,13 @@
         <v>259</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="E115" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
@@ -9568,13 +9597,13 @@
         <v>259</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="E116" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
@@ -9585,13 +9614,13 @@
         <v>259</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="E117" s="2">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
@@ -9602,13 +9631,13 @@
         <v>259</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>103</v>
+        <v>422</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>103</v>
+        <v>423</v>
       </c>
       <c r="E118" s="2">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
@@ -9619,12 +9648,97 @@
         <v>259</v>
       </c>
       <c r="C119" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D119" t="s">
+        <v>425</v>
+      </c>
+      <c r="E119" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E120" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E121" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E122" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E123" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="D124" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="E119" s="2">
+      <c r="E124" s="2">
         <v>14</v>
       </c>
     </row>

</xml_diff>